<commit_message>
fix: precise cell mapping for XLSX template (B4-B18)
</commit_message>
<xml_diff>
--- a/public/templates/template.xlsx
+++ b/public/templates/template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Siddique Akbar\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29668EB3-F8F0-425F-9F53-BA1628CD8363}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D68D7B5A-33D2-4FAD-BEF3-C3D138590859}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -129,7 +129,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -263,33 +263,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -319,12 +297,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -672,10 +644,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -690,119 +662,115 @@
       </c>
       <c r="B1" s="12"/>
     </row>
-    <row r="2" spans="1:2" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="31.5" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A2" s="13"/>
       <c r="B2" s="14"/>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="15"/>
-      <c r="B3" s="16"/>
+    <row r="3" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A3" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="8"/>
     </row>
     <row r="4" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A4" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="8"/>
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2"/>
     </row>
     <row r="5" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B5" s="2"/>
     </row>
     <row r="6" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B6" s="2"/>
     </row>
     <row r="7" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B7" s="2"/>
     </row>
     <row r="8" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" s="2"/>
+      <c r="A8" s="15"/>
+      <c r="B8" s="16"/>
     </row>
     <row r="9" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A9" s="17"/>
-      <c r="B9" s="18"/>
+      <c r="A9" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="10"/>
     </row>
     <row r="10" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A10" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="B10" s="10"/>
+      <c r="A10" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="4"/>
     </row>
     <row r="11" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B11" s="4"/>
     </row>
     <row r="12" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B12" s="4"/>
     </row>
     <row r="13" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A13" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B13" s="4"/>
+      <c r="A13" s="15"/>
+      <c r="B13" s="16"/>
     </row>
     <row r="14" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A14" s="17"/>
-      <c r="B14" s="18"/>
+      <c r="A14" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" s="10"/>
     </row>
     <row r="15" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A15" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B15" s="10"/>
+      <c r="A15" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15" s="4"/>
     </row>
     <row r="16" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B16" s="4"/>
     </row>
     <row r="17" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B17" s="4"/>
     </row>
-    <row r="18" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A18" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B18" s="4"/>
-    </row>
-    <row r="19" spans="1:2" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="5" t="s">
+    <row r="18" spans="1:2" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B19" s="6"/>
+      <c r="B18" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:B3"/>
+    <mergeCell ref="A3:B3"/>
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A13:B13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1 A5:A8 A4 A11:A13 A10 A16:A19 A15 A9 A14" numberStoredAsText="1"/>
+    <ignoredError sqref="A1 A4:A7 A3 A10:A12 A9 A15:A18 A14 A8 A13" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>